<commit_message>
funkcni & nefunkcni pozadavky
</commit_message>
<xml_diff>
--- a/Dokumentace a přílohy/FR.xlsx
+++ b/Dokumentace a přílohy/FR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asher\Desktop\Škola\4 Sem\RSP\Dev\rsproject\Dokumentace a přílohy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jirka\Desktop\Škola\ČVUT\RSP\repository\rsproject\Dokumentace a přílohy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF5B3D2-989A-4F27-90F7-E6F1D1F7A514}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7799ED07-72AB-4C5C-BD4B-8F5294DCFF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="2760" windowWidth="21600" windowHeight="11385" xr2:uid="{BFAFACC6-EB15-4028-A035-B2AA02AC3678}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BFAFACC6-EB15-4028-A035-B2AA02AC3678}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -150,13 +150,13 @@
     <t>Jako uživatel chci odstranit svôůj profil.</t>
   </si>
   <si>
-    <t>Aplikace bude dobře upgradeovatelná.</t>
-  </si>
-  <si>
-    <t>Aplikace bude zvládat příval uživatelů.</t>
-  </si>
-  <si>
     <t>Aplikace bude mít podporu na příštích 5 let.</t>
+  </si>
+  <si>
+    <t>Aplikace bude dobře škálovatelná</t>
+  </si>
+  <si>
+    <t>Aplikace bude zvládat velkou zátěž uživatelů</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -520,21 +520,21 @@
   <dimension ref="B2:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.140625" customWidth="1"/>
-    <col min="3" max="3" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" customWidth="1"/>
+    <col min="3" max="3" width="72.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
     <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
@@ -548,7 +548,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -574,7 +574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -588,13 +588,13 @@
         <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -608,13 +608,13 @@
         <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -628,13 +628,13 @@
         <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -645,7 +645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -656,7 +656,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>21</v>
       </c>
@@ -667,7 +667,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -678,7 +678,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -689,7 +689,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -700,7 +700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>25</v>
       </c>
@@ -711,7 +711,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>26</v>
       </c>
@@ -722,7 +722,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>27</v>
       </c>
@@ -733,7 +733,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>28</v>
       </c>
@@ -744,7 +744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
updated Functional Requirements /still without difficulty in man-days/
</commit_message>
<xml_diff>
--- a/Dokumentace a přílohy/FR.xlsx
+++ b/Dokumentace a přílohy/FR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jirka\Desktop\Škola\ČVUT\RSP\repository\rsproject\Dokumentace a přílohy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asher\Desktop\Škola\4 Sem\RSP\Dev\rsproject\Dokumentace a přílohy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7799ED07-72AB-4C5C-BD4B-8F5294DCFF69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332F30DB-7646-43D2-B9C3-BA4E845A9BBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BFAFACC6-EB15-4028-A035-B2AA02AC3678}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BFAFACC6-EB15-4028-A035-B2AA02AC3678}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Popis</t>
   </si>
@@ -42,45 +42,6 @@
     <t>Priorita</t>
   </si>
   <si>
-    <t>Jako CK chci specifikovat požadavky pro zájemce o zájezd.</t>
-  </si>
-  <si>
-    <t>Jako CK chci upravovat ranking uživatelům.</t>
-  </si>
-  <si>
-    <t>Jako uživatel chci vyhledat, zobrazit, přihlásit k zájezdu.</t>
-  </si>
-  <si>
-    <t>Jako uživatel chci ohodnotit a okomentovat zájezd.</t>
-  </si>
-  <si>
-    <t>Jako uživatel chci vidět svůj profil, hodnocení, achievementy a historií zájezdů.</t>
-  </si>
-  <si>
-    <t>Jako CK chci aby každý uživatel viděl i pro něj nedostupné zájezdy.</t>
-  </si>
-  <si>
-    <t>Jako uživatel chci filtrovat nabídky podle všehomožnýho.</t>
-  </si>
-  <si>
-    <t>Jako uživatel chci upravovat svůj profil.</t>
-  </si>
-  <si>
-    <t>Náročnost</t>
-  </si>
-  <si>
-    <t>Jako uživatel chci přidat své certifikáty a diplomy.</t>
-  </si>
-  <si>
-    <t>Jako uživatel chci odhlášení ze zájezdu.</t>
-  </si>
-  <si>
-    <t>Jako CK chci rozdělit cenu za zájezd na cenu a zálohu.</t>
-  </si>
-  <si>
-    <t>Jako CK chci přidávat a upravovat nabídky.</t>
-  </si>
-  <si>
     <t>FR1</t>
   </si>
   <si>
@@ -126,9 +87,6 @@
     <t>must-to-have</t>
   </si>
   <si>
-    <t>Jako CK chci přidávat a upravovat achievementy.</t>
-  </si>
-  <si>
     <t>nice-to-have</t>
   </si>
   <si>
@@ -147,9 +105,6 @@
     <t>NR3</t>
   </si>
   <si>
-    <t>Jako uživatel chci odstranit svôůj profil.</t>
-  </si>
-  <si>
     <t>Aplikace bude mít podporu na příštích 5 let.</t>
   </si>
   <si>
@@ -157,6 +112,57 @@
   </si>
   <si>
     <t>Aplikace bude zvládat velkou zátěž uživatelů</t>
+  </si>
+  <si>
+    <t>Systém umožní administrátorovi přidávat nové achievementy.</t>
+  </si>
+  <si>
+    <t>Systém umožní administrátorovi specifikovat podmínky pro umožnění účasti na zájezdu.</t>
+  </si>
+  <si>
+    <t>Systém umožní administrátorovi přidat nové zájezdy.</t>
+  </si>
+  <si>
+    <t>Systém umožní administrátorovi upravovat uživatelský ranking.</t>
+  </si>
+  <si>
+    <t>Systém bude zobrazovat uživatelům i zájezdy, které jim nejsou prozatím dostupné.</t>
+  </si>
+  <si>
+    <t>Systém umožní administrátorovi pro každý zájezd určit cenu i zálohu.</t>
+  </si>
+  <si>
+    <t>Systém umožní uživatelům vyhledávání zájezdu podle specifikace destinace, místa, potřebného rankingu pro účast na zájezdu nebo typu zájezdu.</t>
+  </si>
+  <si>
+    <t>Systém umožní uživatelům přidat hodnocení zájezdu, na kterém byli.</t>
+  </si>
+  <si>
+    <t>Systém umožní uživatelům zobrazit si detail profilu (level/rank, achievementy, historií zájezdů)</t>
+  </si>
+  <si>
+    <t>Systém umožní uživatelům upravit si svůj profil.</t>
+  </si>
+  <si>
+    <t>Systém umožní uživatelům přihlášeným na zájezd se ze zájezdu odhlásit.</t>
+  </si>
+  <si>
+    <t>Systém umožní uživatelům přidávat své certifikáty a diplomy.</t>
+  </si>
+  <si>
+    <t>Systém umožní uživatelům odstranit svůj profil.</t>
+  </si>
+  <si>
+    <t>Systém umožní administrátorovi odstranit zájezdy.</t>
+  </si>
+  <si>
+    <t>Náročnost v man-days</t>
+  </si>
+  <si>
+    <t>Systém umožní administrátorovi upravovat zájezdy.</t>
+  </si>
+  <si>
+    <t>FR15</t>
   </si>
 </sst>
 </file>
@@ -205,7 +211,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -221,7 +227,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -517,38 +523,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D96B78F-4FC2-4F7A-8250-8FB9AA372BA8}">
-  <dimension ref="B2:K17"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.109375" customWidth="1"/>
-    <col min="3" max="3" width="72.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" customWidth="1"/>
+    <col min="3" max="3" width="132.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -559,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
         <v>1</v>
@@ -571,188 +578,199 @@
         <v>2</v>
       </c>
       <c r="K3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>